<commit_message>
Auto-committed on 2022/11/08 週二 11:51:42.69
</commit_message>
<xml_diff>
--- a/Program/Other/L9716_底稿_逾放處理催收明細表.xlsx
+++ b/Program/Other/L9716_底稿_逾放處理催收明細表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="YYYMM工作表" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>逾期數</t>
   </si>
@@ -231,14 +231,6 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>HGTCDT</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
-    <t>專辦</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
     <t>用途別</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
@@ -251,8 +243,14 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>篩選</t>
+    <t>核貸金額</t>
     <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>HGTCDT</t>
+  </si>
+  <si>
+    <t>專辦</t>
   </si>
 </sst>
 </file>
@@ -964,9 +962,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="20" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="20" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -975,6 +970,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="20" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1326,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1052"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
@@ -1424,10 +1422,10 @@
       <c r="V1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="13"/>
+      <c r="X1" s="16"/>
       <c r="Y1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4600,10 +4598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU546"/>
+  <dimension ref="A1:AQ546"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -4630,241 +4628,234 @@
     <col min="28" max="28" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.7265625" customWidth="1"/>
-    <col min="43" max="43" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="10" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10" customWidth="1"/>
+    <col min="33" max="33" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.7265625" customWidth="1"/>
+    <col min="42" max="44" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:43" s="15" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="15">
+      <c r="F1" s="14">
         <f>SUBTOTAL(3,F2:F1488)</f>
         <v>0</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="15">
+      <c r="I1" s="14">
         <f>SUBTOTAL(9,I2:I1488)</f>
         <v>0</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AA1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AB1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AC1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AD1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AE1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AF1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AH1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AI1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM1" s="15">
+      <c r="AK1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM1" s="13">
         <f>SUBTOTAL(9,AM2:AM1488)</f>
         <v>0</v>
       </c>
       <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14" t="s">
+      <c r="AO1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AR1" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="AT1" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="AU1" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47">
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" t="str">
         <f>C2&amp;D2&amp;E2</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:43">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">C3&amp;D3&amp;E3</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:43">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:43">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:43">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:43">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:43">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:43">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:43">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:43">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47">
+    <row r="12" spans="1:43">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47">
+    <row r="13" spans="1:43">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47">
+    <row r="14" spans="1:43">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47">
+    <row r="15" spans="1:43">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47">
+    <row r="16" spans="1:43">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
Auto-committed on 2022/11/22 週二 17:26:19.87
</commit_message>
<xml_diff>
--- a/Program/Other/L9716_底稿_逾放處理催收明細表.xlsx
+++ b/Program/Other/L9716_底稿_逾放處理催收明細表.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>逾期數</t>
   </si>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>HGTCDT</t>
-  </si>
-  <si>
-    <t>專辦</t>
   </si>
 </sst>
 </file>
@@ -4598,10 +4595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ546"/>
+  <dimension ref="A1:AN546"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -4633,13 +4630,10 @@
     <col min="34" max="34" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.7265625" customWidth="1"/>
-    <col min="42" max="44" width="10" bestFit="1" customWidth="1"/>
+    <col min="39" max="41" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="15" customFormat="1" ht="30" customHeight="1">
+    <row r="1" spans="1:40" s="15" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>22</v>
       </c>
@@ -4754,108 +4748,100 @@
         <v>59</v>
       </c>
       <c r="AL1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM1" s="13">
-        <f>SUBTOTAL(9,AM2:AM1488)</f>
-        <v>0</v>
-      </c>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AM1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:40">
       <c r="A2" t="str">
         <f>C2&amp;D2&amp;E2</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:40">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">C3&amp;D3&amp;E3</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:40">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:40">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:40">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:40">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:40">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:40">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:40">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:40">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:40">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:40">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:40">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:40">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:40">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>